<commit_message>
+75% winrate against every character
319 games done
</commit_message>
<xml_diff>
--- a/smash_training.xlsx
+++ b/smash_training.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Developpement\smash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D5CF8-BC61-4EDA-9562-52C419E0A2AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D304A2-9D9B-4E14-8EF5-746B6075B823}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30255" yWindow="2400" windowWidth="20910" windowHeight="11835" xr2:uid="{B88D8BEE-BC60-44C6-A929-46D594583A2F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24510" windowHeight="15990" activeTab="1" xr2:uid="{B88D8BEE-BC60-44C6-A929-46D594583A2F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stuff to train" sheetId="1" r:id="rId1"/>
+    <sheet name="Combo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$G$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Stuff to train'!$A$1:$G$30</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="63">
   <si>
     <t>Technique Name</t>
   </si>
@@ -181,13 +182,53 @@
   </si>
   <si>
     <t>Timing : when you are being projected, even before hitting the wall (+ jump !)</t>
+  </si>
+  <si>
+    <t>Moves</t>
+  </si>
+  <si>
+    <t>Lower range</t>
+  </si>
+  <si>
+    <t>Higher range</t>
+  </si>
+  <si>
+    <t>Against light characters (Pichu)</t>
+  </si>
+  <si>
+    <t>Against heavy characters (Bowser)</t>
+  </si>
+  <si>
+    <t>D-Throw</t>
+  </si>
+  <si>
+    <t>Fast Fall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-Air</t>
+  </si>
+  <si>
+    <t>U-Air</t>
+  </si>
+  <si>
+    <t>Damage (Stale ON)</t>
+  </si>
+  <si>
+    <t>1st U-Air : L + C-Stick up + Stick forward (instant)
+Be careful to not buffer it ==&gt; F-Air instead</t>
+  </si>
+  <si>
+    <t>Full Hop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +247,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -417,10 +472,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,22 +538,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -860,10 +932,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B62CDA-92D9-4658-88E6-DA887FC5A079}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -902,7 +973,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -949,7 +1020,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -971,7 +1042,7 @@
       </c>
       <c r="G4" s="18"/>
     </row>
-    <row r="5" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1130,7 @@
       </c>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="9" spans="1:7" ht="19.5" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
@@ -1147,7 +1218,7 @@
       </c>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="13" spans="1:7" ht="19.5" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1213,7 +1284,7 @@
       </c>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="16" spans="1:7" ht="19.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1235,7 +1306,7 @@
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="17" spans="1:7" ht="19.5" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1350,7 @@
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="19" spans="1:7" ht="19.5" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
@@ -1477,7 +1548,7 @@
       </c>
       <c r="G27" s="17"/>
     </row>
-    <row r="28" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="28" spans="1:7" ht="19.5" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1499,7 +1570,7 @@
       </c>
       <c r="G28" s="17"/>
     </row>
-    <row r="29" spans="1:7" ht="19.5" hidden="1" customHeight="1">
+    <row r="29" spans="1:7" ht="19.5" customHeight="1">
       <c r="A29" s="11" t="s">
         <v>32</v>
       </c>
@@ -1544,13 +1615,7 @@
       <c r="G30" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G30" xr:uid="{5D2E021B-D5D6-4FAE-A153-AF23587121EE}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="High"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G30" xr:uid="{5D2E021B-D5D6-4FAE-A153-AF23587121EE}"/>
   <conditionalFormatting sqref="C2:C30">
     <cfRule type="expression" dxfId="8" priority="6">
       <formula>C2="Trick"</formula>
@@ -1577,13 +1642,162 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F30">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>F2="No"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>F2="Yes"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>F2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821DE5B6-3606-417C-903D-25C25C2B037B}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.85546875" defaultRowHeight="18.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="16.85546875" style="1"/>
+    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="82.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0</v>
+      </c>
+      <c r="C3" s="24">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0.45</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>